<commit_message>
adding TC and test data for register page
</commit_message>
<xml_diff>
--- a/test_data/Demo_Web_Shop_manual_TC.xlsx
+++ b/test_data/Demo_Web_Shop_manual_TC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shubham\python_projects\python_selenium_framework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F107F05-F2B7-45A2-AAA2-DB6F1BAA0F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3613DAEA-A581-40AB-8B95-113747AEFEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{0F7B0294-EA83-4638-8023-A9B3120B305A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{0F7B0294-EA83-4638-8023-A9B3120B305A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="147">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -741,9 +741,6 @@
   </si>
   <si>
     <t>passw</t>
-  </si>
-  <si>
-    <t>passwo</t>
   </si>
   <si>
     <t>male</t>
@@ -1723,6 +1720,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="J6:J8"/>
@@ -1731,14 +1736,6 @@
     <mergeCell ref="H9:H11"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2175,8 +2172,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
@@ -2254,7 +2251,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>137</v>
@@ -2283,7 +2280,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>137</v>
@@ -2314,7 +2311,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>142</v>
@@ -2676,10 +2673,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C059C7-4640-4A99-A9A9-19193BC4DF76}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15"/>
@@ -2687,17 +2684,12 @@
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="42.42578125" customWidth="1"/>
-    <col min="11" max="11" width="50.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
         <v>120</v>
       </c>
@@ -2708,33 +2700,15 @@
         <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>142</v>
@@ -2742,337 +2716,182 @@
       <c r="C2" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>143</v>
+      <c r="D2" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="1:11">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{154D9BA1-95D7-4CF2-BD48-72465F1168DC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>